<commit_message>
Screentshot added but cant show in report
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData_v2.xlsx
+++ b/src/test/resources/testData/TestData_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git_Repo\WebAutomationAssesment\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFB636B-A39F-4353-B550-4BA600A0055E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EB31BC-81FF-46DA-9E89-5E168A3719FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20460" yWindow="495" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
     <t>username=automate.cheq@yopmail.com,password=Automation@2025</t>
   </si>
   <si>
-    <t>username=invalid@email.com,password=wer</t>
+    <t>username=invalid@email.com,password=wer43345454</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="3" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
   </cols>
@@ -479,7 +480,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
first commit in feature-extend
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData_v2.xlsx
+++ b/src/test/resources/testData/TestData_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git_Repo\WebAutomationAssesment\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7254EF2-6A48-4CC4-BBD5-42845ECD861D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43A8477-9802-40C8-9D47-3DCDBDD07E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Select Event for March 17, 2025</t>
   </si>
   <si>
-    <t>Automation Horizon</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -130,16 +127,22 @@
     <t>Select Event for March 19, 2025</t>
   </si>
   <si>
-    <t>Event A</t>
-  </si>
-  <si>
     <t>No event for March 16, 2025</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>eid event</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>sony proibar</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,13 +660,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -683,13 +686,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,16 +700,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>13</v>
@@ -717,19 +720,19 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="5">
-        <v>45735</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>